<commit_message>
Created graphs for Percentage Feature Creators
</commit_message>
<xml_diff>
--- a/tests/xlsxfilereadertests/testfile2.xlsx
+++ b/tests/xlsxfilereadertests/testfile2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmyshong/Desktop/NYUCS/AIfSR/2021-fall-unsupervised-learning/tests/xlsxfilereadertests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38215D89-9DEF-C047-9BCD-25A02464CCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6E36D0-B6D1-A647-A3E4-FDA140B4B99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="3340" windowWidth="27640" windowHeight="16540" xr2:uid="{5ACA507C-7F00-8747-AA99-C118D805E904}"/>
+    <workbookView xWindow="1160" yWindow="1460" windowWidth="27640" windowHeight="16540" xr2:uid="{5ACA507C-7F00-8747-AA99-C118D805E904}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,19 +465,19 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I3">
         <v>7</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K3">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>